<commit_message>
EPBDS-2524 Call one method several times when calling it with the same signature, but with one of the arguments as array
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/binding/ArrayMethodsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/binding/ArrayMethodsTest.xlsx
@@ -131,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +171,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,15 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -229,6 +238,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -525,25 +540,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="17" max="17" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:12">
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -554,7 +569,7 @@
       </c>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -565,15 +580,15 @@
       </c>
     </row>
     <row r="10" spans="2:12">
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -590,7 +605,7 @@
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" t="s">
+      <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -607,77 +622,77 @@
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" t="s">
+      <c r="B16" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" t="s">
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" t="s">
+      <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" t="s">
+      <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" t="s">
+      <c r="B24" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" t="s">
+      <c r="B28" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" t="s">
+      <c r="B32" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:17">
-      <c r="B33" t="s">
+      <c r="B33" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:17">
-      <c r="Q35" t="s">
+      <c r="Q35" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" spans="2:17">
-      <c r="Q36" t="s">
+      <c r="Q36" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="60" customHeight="1">
-      <c r="Q37" s="5" t="s">
+      <c r="Q37" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="2:17">
-      <c r="B42" t="s">
+      <c r="B42" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:17" ht="81" customHeight="1">
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="11" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-3240 fixed calling multiple arguments method of void type
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/binding/ArrayMethodsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/binding/ArrayMethodsTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="18195" windowHeight="7740"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="18195" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Datatype PersonType</t>
   </si>
@@ -110,12 +110,77 @@
 intMas[1] = 7;
 return intTest(intArrayTest(intMas));</t>
   </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <r>
+      <t>TBasic void TBasicCall</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>Method void test(int a)</t>
+  </si>
+  <si>
+    <t>a++;</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Operation Execution</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>new int[]{1,2,3}</t>
+  </si>
+  <si>
+    <t>test(array)</t>
+  </si>
+  <si>
+    <t>Call multi arguments</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,8 +195,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +286,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="29"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -219,37 +343,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -328,6 +509,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -362,6 +544,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -537,28 +720,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.5703125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="17" max="17" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12">
-      <c r="I4" s="5" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:12">
-      <c r="B5" s="10" t="s">
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -568,8 +751,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -579,16 +762,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
-      <c r="I10" s="6" t="s">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="2:12">
-      <c r="B11" s="10" t="s">
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -604,8 +787,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
-      <c r="B12" s="11" t="s">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -621,78 +804,78 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="10" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="11" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="10" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="11" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="10" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:17">
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:17">
-      <c r="Q35" s="8" t="s">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q35" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="2:17">
-      <c r="Q36" s="8" t="s">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q36" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:17" ht="60" customHeight="1">
-      <c r="Q37" s="9" t="s">
+    <row r="37" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="2:17">
-      <c r="B42" s="10" t="s">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="2:17" ht="81" customHeight="1">
-      <c r="B43" s="11" t="s">
+    <row r="43" spans="2:17" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -707,24 +890,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="18"/>
+      <c r="D9" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>